<commit_message>
Modified reference data replacement logic
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCaseData1.xlsx
+++ b/src/main/resources/TestCaseData1.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="Reference" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -111,36 +111,12 @@
     <t>tc1r1c5</t>
   </si>
   <si>
-    <t>tc1r2c3</t>
-  </si>
-  <si>
-    <t>tc1r2c4</t>
-  </si>
-  <si>
     <t>tc1r2c5</t>
   </si>
   <si>
-    <t>tc1r3c1</t>
-  </si>
-  <si>
-    <t>tc1r3c2</t>
-  </si>
-  <si>
-    <t>tc1r3c3</t>
-  </si>
-  <si>
-    <t>tc1r3c4</t>
-  </si>
-  <si>
     <t>tc1r3c5</t>
   </si>
   <si>
-    <t>tc2r1c1</t>
-  </si>
-  <si>
-    <t>tc2r1c2</t>
-  </si>
-  <si>
     <t>tc2r2c1</t>
   </si>
   <si>
@@ -214,12 +190,37 @@
   </si>
   <si>
     <t>swapnil</t>
+  </si>
+  <si>
+    <t>welcome ${userName}!</t>
+  </si>
+  <si>
+    <t>${userName} last logged in at ${myDate}</t>
+  </si>
+  <si>
+    <t>${userFirstName}</t>
+  </si>
+  <si>
+    <t>${userLastName}</t>
+  </si>
+  <si>
+    <t>sonar</t>
+  </si>
+  <si>
+    <t>${userFullName}</t>
+  </si>
+  <si>
+    <t>welcome ${userFullName}!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -319,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -330,8 +331,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -707,20 +715,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -749,11 +759,11 @@
       <c r="B3" s="2">
         <v>11</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="12">
         <v>12.2</v>
       </c>
-      <c r="D3" s="8">
-        <v>43202</v>
+      <c r="D3" s="9">
+        <v>43203</v>
       </c>
       <c r="E3" s="2" t="b">
         <v>1</v>
@@ -766,58 +776,58 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>62</v>
+      <c r="B4" s="2">
+        <v>22</v>
+      </c>
+      <c r="C4" s="12">
+        <v>45.89</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>33</v>
+      </c>
+      <c r="C5" s="12">
+        <v>78.224000000000004</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -841,10 +851,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -855,35 +865,35 @@
         <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -913,22 +923,22 @@
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -936,22 +946,22 @@
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -959,34 +969,34 @@
         <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -998,43 +1008,69 @@
     <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>64</v>
+      <c r="A1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="11">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="8">
-        <v>43191</v>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="10" t="str">
+        <f>CONCATENATE(B4," ",B5)</f>
+        <v>swapnil sonar</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test case worksheet
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCaseData1.xlsx
+++ b/src/main/resources/TestCaseData1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -646,7 +646,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -708,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1018,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
updated test case data worksheet
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCaseData1.xlsx
+++ b/src/main/resources/TestCaseData1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -646,9 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -710,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,9 +1016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>